<commit_message>
feat: Git ignore file
</commit_message>
<xml_diff>
--- a/templates/template_mon.xlsx
+++ b/templates/template_mon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63737ae24bd6586a/Documentos/Programas/python/autoRancho/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Documentos\Programas\python\autoRancho\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{74EB567F-66BE-4AC6-8ADC-EEB6383C8652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF002AC8-5055-4E32-AB6F-D0267F19D7BF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67707026-175A-425E-84FA-22586749C21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7DF6366A-B2EB-4283-B8F8-84095FA92494}"/>
   </bookViews>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="59">
   <si>
     <t>2º ESQUADRÃO DE CARROS DE COMBATE</t>
   </si>
@@ -368,132 +368,42 @@
     <t>-</t>
   </si>
   <si>
-    <t>BERTAZZO</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>R.SOARES</t>
-  </si>
-  <si>
-    <t>SCHRÖDER</t>
-  </si>
-  <si>
-    <t>NOGUEIRA</t>
-  </si>
-  <si>
     <t>ASP OF</t>
   </si>
   <si>
-    <t>VICENTE</t>
-  </si>
-  <si>
-    <t>ALEXANDRE</t>
-  </si>
-  <si>
     <t>TOTAL OFICIAIS</t>
   </si>
   <si>
-    <t>EGGRES</t>
-  </si>
-  <si>
-    <t>SARAIVA</t>
-  </si>
-  <si>
     <t>ST / SGT</t>
   </si>
   <si>
-    <t xml:space="preserve"> DIAS</t>
-  </si>
-  <si>
-    <t>CALDEIRA</t>
-  </si>
-  <si>
     <t>ST</t>
   </si>
   <si>
-    <t>AUREO</t>
-  </si>
-  <si>
-    <t>BASTOS</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>1º SGT</t>
   </si>
   <si>
-    <t>KESSNER</t>
-  </si>
-  <si>
-    <t>ZIANI</t>
-  </si>
-  <si>
     <t>2º SGT</t>
   </si>
   <si>
-    <t>MACHADO</t>
-  </si>
-  <si>
-    <t>EDUARDO MORAIS</t>
-  </si>
-  <si>
-    <t>NETO</t>
-  </si>
-  <si>
-    <t>OLIVEIRA</t>
-  </si>
-  <si>
     <t>3º SGT</t>
   </si>
   <si>
-    <t>RISSO</t>
-  </si>
-  <si>
-    <t>BRAGA</t>
-  </si>
-  <si>
     <t>3° SGT</t>
   </si>
   <si>
-    <t>SARAÇOL</t>
-  </si>
-  <si>
-    <t>SARAIVA SOARES</t>
-  </si>
-  <si>
-    <t>WHUESLEN</t>
-  </si>
-  <si>
-    <t>ANDERSON</t>
-  </si>
-  <si>
-    <t>VAZ</t>
-  </si>
-  <si>
-    <t>VARGAS</t>
-  </si>
-  <si>
-    <t>PIERESAN</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -</t>
   </si>
   <si>
-    <t>LAMANCHA</t>
-  </si>
-  <si>
-    <t>BORTOLI</t>
-  </si>
-  <si>
     <t>TOTAL SD EP</t>
   </si>
   <si>
-    <t>VITOR SOARES</t>
-  </si>
-  <si>
     <t>TOTAL ST / SGT</t>
   </si>
   <si>
@@ -503,175 +413,31 @@
     <t>CB EP</t>
   </si>
   <si>
-    <t>DEBORTOLI</t>
-  </si>
-  <si>
-    <t>KEVIN</t>
-  </si>
-  <si>
-    <t>SOUZA</t>
-  </si>
-  <si>
-    <t>ALVIANA</t>
-  </si>
-  <si>
-    <t>FLORES</t>
-  </si>
-  <si>
-    <t>SAUCEDA</t>
-  </si>
-  <si>
-    <t>SCARPARO</t>
-  </si>
-  <si>
-    <t>RICHARD</t>
-  </si>
-  <si>
-    <t>SOUZA SILVA</t>
-  </si>
-  <si>
-    <t>DO AMARAL</t>
-  </si>
-  <si>
-    <t>GREINER</t>
-  </si>
-  <si>
-    <t>HILGERT</t>
-  </si>
-  <si>
-    <t>GUILHERME SALLES</t>
-  </si>
-  <si>
-    <t>CEZILIO</t>
-  </si>
-  <si>
-    <t>GIL</t>
-  </si>
-  <si>
-    <t>SANGUINETE</t>
-  </si>
-  <si>
-    <t>LUI</t>
-  </si>
-  <si>
-    <t>DOTTO</t>
-  </si>
-  <si>
-    <t>ASMAN</t>
-  </si>
-  <si>
-    <t>REZENDE</t>
-  </si>
-  <si>
-    <t>JULIO MORAES</t>
-  </si>
-  <si>
-    <t>ANDREI</t>
-  </si>
-  <si>
-    <t>LUBENOW</t>
-  </si>
-  <si>
-    <t>BORGES</t>
-  </si>
-  <si>
-    <t>K.MOREIRA</t>
-  </si>
-  <si>
-    <t>ANDRÉ</t>
-  </si>
-  <si>
-    <t>EUZÉBIO</t>
-  </si>
-  <si>
-    <t>VIEIRA</t>
-  </si>
-  <si>
-    <t>BERTÓGLIO</t>
-  </si>
-  <si>
-    <t>FIUZA</t>
-  </si>
-  <si>
-    <t>LUAN MELO</t>
-  </si>
-  <si>
-    <t>BRITO</t>
-  </si>
-  <si>
-    <t>L. DIAS</t>
-  </si>
-  <si>
-    <t>ESTIGARRIBIA</t>
-  </si>
-  <si>
-    <t>MENDES SILVA</t>
-  </si>
-  <si>
-    <t>DOS SANTOS</t>
-  </si>
-  <si>
-    <t>LUIZ SILVA</t>
-  </si>
-  <si>
     <t>TOTAL CB</t>
   </si>
   <si>
-    <t>HENRIQUE SILVA</t>
-  </si>
-  <si>
-    <t>DO AMARANTE</t>
-  </si>
-  <si>
     <t>SERVIÇO</t>
   </si>
   <si>
-    <t>STIEVEN</t>
-  </si>
-  <si>
-    <t>SPIECKERT</t>
-  </si>
-  <si>
     <t>PLANTÃO 1</t>
   </si>
   <si>
-    <t>DAL LAGO</t>
-  </si>
-  <si>
     <t>PLANTÃO 2</t>
   </si>
   <si>
-    <t>DE LIMA</t>
-  </si>
-  <si>
     <t>PLANTÃO 3</t>
   </si>
   <si>
-    <t>G. NUNES</t>
-  </si>
-  <si>
     <t>GUARDA 1</t>
   </si>
   <si>
-    <t>GUSTAVO SANTOS</t>
-  </si>
-  <si>
     <t>GUARDA 2</t>
   </si>
   <si>
-    <t>TALISSON</t>
-  </si>
-  <si>
     <t>GUARDA 3</t>
   </si>
   <si>
-    <t>BARCELLOS</t>
-  </si>
-  <si>
     <t>GUARDA 4</t>
-  </si>
-  <si>
-    <t>VITOR BORGES</t>
   </si>
   <si>
     <t>PAIOL 1</t>
@@ -756,7 +522,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.00&quot; &quot;;#,##0.00&quot; &quot;;&quot;-&quot;#&quot; &quot;;@&quot; &quot;"/>
     <numFmt numFmtId="169" formatCode="[$R$-416]&quot; &quot;#,##0.00;[Red]&quot;-&quot;[$R$-416]&quot; &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -968,6 +734,22 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1230,7 +1012,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1335,30 +1117,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1366,32 +1124,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1405,7 +1159,43 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Accent" xfId="1" xr:uid="{498CB7F5-00C3-4F6D-855E-942D03B59CA6}"/>
@@ -1858,8 +1648,8 @@
   </sheetPr>
   <dimension ref="A1:AS89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O21" sqref="O6:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1889,97 +1679,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="42.75" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
       <c r="AP1" s="1"/>
     </row>
     <row r="2" spans="1:45" ht="43.8">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
       <c r="AP2" s="1"/>
     </row>
     <row r="3" spans="1:45" ht="16.8">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43" t="str">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48" t="str">
         <f>LEFT(UPPER(TEXT(A3,"dddd")),1)&amp;RIGHT(LOWER(TEXT(A3,"dddd")), LEN(TEXT(A3,"dddd"))-1)</f>
         <v>Sábado</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="M3" s="42">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="M3" s="47">
         <f>(A3)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="42"/>
-      <c r="O3" s="43" t="str">
+      <c r="N3" s="47"/>
+      <c r="O3" s="48" t="str">
         <f>LEFT(UPPER(TEXT(M3,"dddd")),1)&amp;RIGHT(LOWER(TEXT(M3,"dddd")), LEN(TEXT(M3,"dddd"))-1)</f>
         <v>Sábado</v>
       </c>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
       <c r="AR3" s="2"/>
     </row>
     <row r="4" spans="1:45">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="M4" s="40" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="M4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
       <c r="AR4" s="2"/>
     </row>
     <row r="5" spans="1:45">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2018,11 +1808,9 @@
       <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2032,12 +1820,10 @@
       <c r="N6" s="7">
         <v>304</v>
       </c>
-      <c r="O6" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="O6" s="64"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R6" s="7"/>
     </row>
@@ -2048,12 +1834,10 @@
       <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F7" s="6"/>
       <c r="M7" s="9" t="s">
@@ -2062,26 +1846,22 @@
       <c r="N7" s="9">
         <v>309</v>
       </c>
-      <c r="O7" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="O7" s="65"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
     </row>
     <row r="8" spans="1:45">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F8" s="6"/>
       <c r="M8" s="7" t="s">
@@ -2090,21 +1870,19 @@
       <c r="N8" s="7">
         <v>314</v>
       </c>
-      <c r="O8" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="O8" s="66"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:45" ht="16.8">
-      <c r="A9" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
+      <c r="A9" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="11">
         <f>COUNTIF(D6:D8,"X")</f>
         <v>0</v>
@@ -2123,50 +1901,43 @@
       <c r="N9" s="9">
         <v>322</v>
       </c>
-      <c r="O9" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="O9" s="65"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R9" s="9"/>
     </row>
     <row r="10" spans="1:45" ht="16.8" customHeight="1">
-      <c r="K10" s="64"/>
       <c r="M10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N10" s="7">
         <v>347</v>
       </c>
-      <c r="O10" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="O10" s="66"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:45" ht="16.8" customHeight="1">
-      <c r="A11" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
+      <c r="A11" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
       <c r="M11" s="9" t="s">
         <v>2</v>
       </c>
       <c r="N11" s="9">
         <v>363</v>
       </c>
-      <c r="O11" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="O11" s="65"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
@@ -2194,28 +1965,24 @@
       <c r="N12" s="7">
         <v>372</v>
       </c>
-      <c r="O12" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="O12" s="66"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:45" ht="14.4" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F13" s="9"/>
       <c r="M13" s="9" t="s">
@@ -2224,28 +1991,24 @@
       <c r="N13" s="9">
         <v>379</v>
       </c>
-      <c r="O13" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="O13" s="65"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R13" s="9"/>
     </row>
     <row r="14" spans="1:45" ht="14.4" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B14" s="7">
         <v>3</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F14" s="7"/>
       <c r="M14" s="7" t="s">
@@ -2254,29 +2017,25 @@
       <c r="N14" s="7">
         <v>382</v>
       </c>
-      <c r="O14" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="O14" s="66"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R14" s="7"/>
       <c r="AS14" s="12"/>
     </row>
     <row r="15" spans="1:45">
       <c r="A15" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B15" s="9">
         <v>7</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F15" s="9"/>
       <c r="M15" s="9" t="s">
@@ -2285,26 +2044,22 @@
       <c r="N15" s="9">
         <v>384</v>
       </c>
-      <c r="O15" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="O15" s="65"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="AS15" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:45">
       <c r="A16" s="7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B16" s="7">
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2314,9 +2069,7 @@
       <c r="N16" s="7">
         <v>390</v>
       </c>
-      <c r="O16" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="O16" s="66"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
@@ -2324,17 +2077,15 @@
     </row>
     <row r="17" spans="1:45">
       <c r="A17" s="6" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B17" s="9">
         <v>15</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F17" s="6"/>
       <c r="M17" s="9" t="s">
@@ -2343,9 +2094,7 @@
       <c r="N17" s="9">
         <v>398</v>
       </c>
-      <c r="O17" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="O17" s="65"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
@@ -2353,14 +2102,12 @@
     </row>
     <row r="18" spans="1:45">
       <c r="A18" s="7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B18" s="7">
         <v>22</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2370,9 +2117,7 @@
       <c r="N18" s="7">
         <v>404</v>
       </c>
-      <c r="O18" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="O18" s="66"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
@@ -2380,17 +2125,15 @@
     </row>
     <row r="19" spans="1:45">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B19" s="9">
         <v>35</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F19" s="6"/>
       <c r="M19" s="9" t="s">
@@ -2399,29 +2142,25 @@
       <c r="N19" s="9">
         <v>405</v>
       </c>
-      <c r="O19" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="O19" s="65"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R19" s="9"/>
       <c r="AS19" s="12"/>
     </row>
     <row r="20" spans="1:45">
       <c r="A20" s="7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B20" s="7">
         <v>41</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F20" s="7"/>
       <c r="M20" s="7" t="s">
@@ -2430,9 +2169,7 @@
       <c r="N20" s="7">
         <v>411</v>
       </c>
-      <c r="O20" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="O20" s="66"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
@@ -2440,55 +2177,49 @@
     </row>
     <row r="21" spans="1:45">
       <c r="A21" s="6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B21" s="6">
         <v>51</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>48</v>
-      </c>
+      <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F21" s="6"/>
       <c r="M21" s="9" t="s">
         <v>2</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>50</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="O21" s="65"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R21" s="9"/>
       <c r="AS21" s="12"/>
     </row>
     <row r="22" spans="1:45" ht="16.8">
       <c r="A22" s="7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7">
         <v>54</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="C22" s="8"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="M22" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
+      <c r="M22" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
       <c r="P22" s="11">
         <f>COUNTIF(P6:P21,"X")</f>
         <v>0</v>
@@ -2505,27 +2236,25 @@
     </row>
     <row r="23" spans="1:45">
       <c r="A23" s="6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B23" s="6">
         <v>71</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F23" s="6"/>
       <c r="AS23" s="12"/>
     </row>
     <row r="24" spans="1:45" ht="16.8">
-      <c r="A24" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
+      <c r="A24" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="11">
         <f>COUNTIF(D12:D23,"X")</f>
         <v>1</v>
@@ -2539,14 +2268,14 @@
         <v>0</v>
       </c>
       <c r="K24" s="13"/>
-      <c r="M24" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
+      <c r="M24" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" s="45"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
       <c r="AS24" s="12"/>
     </row>
     <row r="25" spans="1:45">
@@ -2569,27 +2298,25 @@
         <v>7</v>
       </c>
       <c r="AS25" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:45">
-      <c r="A26" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="A26" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
       <c r="M26" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N26" s="7">
         <v>500</v>
       </c>
-      <c r="O26" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="O26" s="7"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
@@ -2615,14 +2342,12 @@
         <v>7</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N27" s="9">
         <v>501</v>
       </c>
-      <c r="O27" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
@@ -2630,26 +2355,22 @@
     </row>
     <row r="28" spans="1:45">
       <c r="A28" s="15" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B28" s="16">
         <v>102</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>59</v>
-      </c>
+      <c r="C28" s="16"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="M28" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N28" s="7">
         <v>502</v>
       </c>
-      <c r="O28" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="O28" s="7"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
@@ -2657,57 +2378,49 @@
     </row>
     <row r="29" spans="1:45">
       <c r="A29" s="17" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B29" s="8">
         <v>105</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="C29" s="8"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F29" s="7"/>
       <c r="M29" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N29" s="9">
         <v>503</v>
       </c>
-      <c r="O29" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="O29" s="6"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="AS29" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:45">
       <c r="A30" s="15" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B30" s="16">
         <v>108</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>62</v>
-      </c>
+      <c r="C30" s="16"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="M30" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N30" s="7">
         <v>504</v>
       </c>
-      <c r="O30" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
@@ -2715,146 +2428,126 @@
     </row>
     <row r="31" spans="1:45">
       <c r="A31" s="17" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B31" s="7">
         <v>116</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F31" s="7"/>
       <c r="M31" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N31" s="9">
         <v>505</v>
       </c>
-      <c r="O31" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
       <c r="AS31" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:45">
       <c r="A32" s="15" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B32" s="9">
         <v>117</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="M32" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N32" s="7">
         <v>516</v>
       </c>
-      <c r="O32" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
       <c r="AS32" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:45">
       <c r="A33" s="17" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B33" s="8">
         <v>129</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>68</v>
-      </c>
+      <c r="C33" s="8"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="M33" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N33" s="9">
         <v>506</v>
       </c>
-      <c r="O33" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
       <c r="AS33" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:45">
       <c r="A34" s="15" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B34" s="9">
         <v>139</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>70</v>
-      </c>
+      <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="M34" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N34" s="7">
         <v>507</v>
       </c>
-      <c r="O34" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="O34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
       <c r="AS34" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:45">
       <c r="A35" s="17" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B35" s="7">
         <v>151</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F35" s="7"/>
       <c r="M35" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N35" s="9">
         <v>508</v>
       </c>
-      <c r="O35" s="6" t="s">
-        <v>73</v>
-      </c>
+      <c r="O35" s="6"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
@@ -2862,28 +2555,24 @@
     </row>
     <row r="36" spans="1:45">
       <c r="A36" s="15" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B36" s="9">
         <v>154</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>74</v>
-      </c>
+      <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F36" s="9"/>
       <c r="M36" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N36" s="9">
         <v>510</v>
       </c>
-      <c r="O36" s="6" t="s">
-        <v>75</v>
-      </c>
+      <c r="O36" s="6"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
@@ -2891,28 +2580,24 @@
     </row>
     <row r="37" spans="1:45">
       <c r="A37" s="17" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B37" s="7">
         <v>161</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>76</v>
-      </c>
+      <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F37" s="7"/>
       <c r="M37" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N37" s="7">
         <v>511</v>
       </c>
-      <c r="O37" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="O37" s="7"/>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="7"/>
@@ -2920,243 +2605,211 @@
     </row>
     <row r="38" spans="1:45">
       <c r="A38" s="9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B38" s="6">
         <v>162</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F38" s="9"/>
       <c r="M38" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N38" s="9">
         <v>512</v>
       </c>
-      <c r="O38" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="O38" s="6"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
       <c r="AS38" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:45">
       <c r="A39" s="7" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B39" s="7">
         <v>163</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>80</v>
-      </c>
+      <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F39" s="7"/>
       <c r="M39" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N39" s="7">
         <v>513</v>
       </c>
-      <c r="O39" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="O39" s="7"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
       <c r="AS39" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:45">
       <c r="A40" s="9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B40" s="9">
         <v>179</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>82</v>
-      </c>
+      <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F40" s="9"/>
       <c r="M40" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N40" s="9">
         <v>514</v>
       </c>
-      <c r="O40" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="O40" s="6"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
       <c r="AS40" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:45">
       <c r="A41" s="9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B41" s="9">
         <v>185</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>84</v>
-      </c>
+      <c r="C41" s="18"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F41" s="9"/>
       <c r="M41" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N41" s="7">
         <v>515</v>
       </c>
-      <c r="O41" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="O41" s="7"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
     </row>
     <row r="42" spans="1:45">
       <c r="A42" s="7" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B42" s="8">
         <v>198</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="C42" s="8"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F42" s="7"/>
       <c r="M42" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N42" s="9">
         <v>517</v>
       </c>
-      <c r="O42" s="6" t="s">
-        <v>87</v>
-      </c>
+      <c r="O42" s="6"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
     </row>
     <row r="43" spans="1:45">
       <c r="A43" s="9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B43" s="9">
         <v>205</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>88</v>
-      </c>
+      <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F43" s="9"/>
       <c r="M43" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N43" s="7">
         <v>518</v>
       </c>
-      <c r="O43" s="7" t="s">
-        <v>89</v>
-      </c>
+      <c r="O43" s="7"/>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
     </row>
     <row r="44" spans="1:45">
       <c r="A44" s="7" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B44" s="8">
         <v>206</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>90</v>
-      </c>
+      <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F44" s="7"/>
       <c r="M44" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N44" s="9">
         <v>519</v>
       </c>
-      <c r="O44" s="6" t="s">
-        <v>91</v>
-      </c>
+      <c r="O44" s="6"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
     </row>
     <row r="45" spans="1:45">
       <c r="A45" s="9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B45" s="9">
         <v>214</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F45" s="9"/>
       <c r="M45" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N45" s="7">
         <v>520</v>
       </c>
-      <c r="O45" s="7" t="s">
-        <v>93</v>
-      </c>
+      <c r="O45" s="7"/>
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
     </row>
     <row r="46" spans="1:45" ht="16.8">
-      <c r="A46" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
+      <c r="A46" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
       <c r="D46" s="11">
         <f>COUNTIF(D28:D45,"X")</f>
         <v>0</v>
@@ -3170,50 +2823,44 @@
         <v>0</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N46" s="9">
         <v>521</v>
       </c>
-      <c r="O46" s="6" t="s">
-        <v>95</v>
-      </c>
+      <c r="O46" s="6"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
     </row>
     <row r="47" spans="1:45">
       <c r="M47" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N47" s="7">
         <v>522</v>
       </c>
-      <c r="O47" s="7" t="s">
-        <v>96</v>
-      </c>
+      <c r="O47" s="7"/>
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
       <c r="R47" s="7"/>
     </row>
     <row r="48" spans="1:45">
-      <c r="A48" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
+      <c r="A48" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
       <c r="M48" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N48" s="9">
         <v>523</v>
       </c>
-      <c r="O48" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="O48" s="6"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
@@ -3236,250 +2883,234 @@
         <v>7</v>
       </c>
       <c r="M49" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N49" s="7">
         <v>524</v>
       </c>
-      <c r="O49" s="7" t="s">
-        <v>99</v>
-      </c>
+      <c r="O49" s="7"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="7"/>
     </row>
     <row r="50" spans="1:18">
-      <c r="A50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="44"/>
+      <c r="A50" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="41"/>
       <c r="C50" s="6" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N50" s="9">
         <v>525</v>
       </c>
-      <c r="O50" s="6" t="s">
-        <v>101</v>
-      </c>
+      <c r="O50" s="6"/>
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="44"/>
+      <c r="A51" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="41"/>
       <c r="C51" s="6" t="s">
-        <v>102</v>
+        <v>30</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M51" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N51" s="7">
         <v>526</v>
       </c>
-      <c r="O51" s="7" t="s">
-        <v>103</v>
-      </c>
+      <c r="O51" s="7"/>
       <c r="P51" s="7"/>
       <c r="Q51" s="7"/>
       <c r="R51" s="7"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="44"/>
+      <c r="A52" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="41"/>
       <c r="C52" s="6" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N52" s="9">
         <v>527</v>
       </c>
-      <c r="O52" s="6" t="s">
-        <v>105</v>
-      </c>
+      <c r="O52" s="6"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="44"/>
+      <c r="A53" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="41"/>
       <c r="C53" s="6" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M53" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N53" s="7">
         <v>528</v>
       </c>
-      <c r="O53" s="7" t="s">
-        <v>107</v>
-      </c>
+      <c r="O53" s="7"/>
       <c r="P53" s="7"/>
       <c r="Q53" s="7"/>
       <c r="R53" s="7"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="44"/>
+      <c r="A54" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="41"/>
       <c r="C54" s="6" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N54" s="9">
         <v>529</v>
       </c>
-      <c r="O54" s="6" t="s">
-        <v>109</v>
-      </c>
+      <c r="O54" s="6"/>
       <c r="P54" s="6"/>
       <c r="Q54" s="6"/>
       <c r="R54" s="6"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" s="44"/>
+      <c r="A55" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="41"/>
       <c r="C55" s="6" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M55" s="7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N55" s="7">
         <v>530</v>
       </c>
-      <c r="O55" s="7" t="s">
-        <v>111</v>
-      </c>
+      <c r="O55" s="7"/>
       <c r="P55" s="7"/>
       <c r="Q55" s="7"/>
       <c r="R55" s="7"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="44"/>
+      <c r="A56" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="41"/>
       <c r="C56" s="6" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N56" s="9">
         <v>531</v>
       </c>
-      <c r="O56" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="O56" s="6"/>
       <c r="P56" s="6"/>
       <c r="Q56" s="6"/>
       <c r="R56" s="6"/>
     </row>
     <row r="57" spans="1:18" ht="16.8">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="44"/>
+      <c r="B57" s="41"/>
       <c r="C57" s="6" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M57" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="N57" s="47"/>
-      <c r="O57" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="M57" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="N57" s="39"/>
+      <c r="O57" s="39"/>
       <c r="P57" s="11">
         <f>COUNTIF(P26:P56,"X")</f>
         <v>0</v>
@@ -3494,11 +3125,11 @@
       </c>
     </row>
     <row r="58" spans="1:18" ht="16.8">
-      <c r="A58" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
+      <c r="A58" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
       <c r="D58" s="10">
         <f>COUNTIF(D50:D57,"X")</f>
         <v>8</v>
@@ -3513,29 +3144,27 @@
       </c>
     </row>
     <row r="64" spans="1:18">
-      <c r="O64" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="P64" s="48"/>
+      <c r="O64" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P64" s="40"/>
     </row>
     <row r="65" spans="15:16">
-      <c r="O65" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="P65" s="48"/>
+      <c r="O65" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="P65" s="40"/>
     </row>
     <row r="89" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="O64:P64"/>
-    <mergeCell ref="O65:P65"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="M57:O57"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="A1:R2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:R3"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:C9"/>
@@ -3548,13 +3177,15 @@
     <mergeCell ref="A48:F48"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="M4:R4"/>
-    <mergeCell ref="A1:R2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="O64:P64"/>
+    <mergeCell ref="O65:P65"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="M57:O57"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3576,13 +3207,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A1" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="A1" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" hidden="1" customHeight="1">
       <c r="A2" s="21"/>
@@ -3600,47 +3231,47 @@
     </row>
     <row r="4" spans="1:12" ht="63" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
+        <v>41</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:12" ht="26.1" customHeight="1">
-      <c r="A5" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="A5" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
     </row>
     <row r="6" spans="1:12" ht="26.1" customHeight="1">
-      <c r="A6" s="51"/>
-      <c r="B6" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
     </row>
     <row r="7" spans="1:12" ht="26.1" customHeight="1">
-      <c r="A7" s="51"/>
-      <c r="B7" s="54">
+      <c r="A7" s="60"/>
+      <c r="B7" s="63">
         <f>(Planilha1!A3)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:12" ht="17.850000000000001" customHeight="1">
-      <c r="A8" s="51"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -3648,201 +3279,201 @@
       <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A9" s="51"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="23" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>125</v>
+        <v>47</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>127</v>
+        <v>49</v>
       </c>
       <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12" ht="32.85" customHeight="1">
-      <c r="A10" s="56" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="57">
+      <c r="A10" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="56">
         <f>SUM(Planilha1!D9)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="57">
+      <c r="C10" s="56">
         <f>SUM(Planilha1!E9)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="57">
+      <c r="D10" s="56">
         <f>SUM(Planilha1!F9)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="57">
         <f>SUM(A10:D10)</f>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A11" s="56"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
     </row>
     <row r="12" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A12" s="56"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="57"/>
     </row>
     <row r="13" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A13" s="56"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A14" s="56"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
     </row>
     <row r="15" spans="1:12" ht="13.35" customHeight="1">
-      <c r="A15" s="56"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="58"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
     </row>
     <row r="16" spans="1:12" ht="30.45" customHeight="1">
-      <c r="A16" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" s="57">
+      <c r="A16" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="56">
         <f>SUM(Planilha1!D24)</f>
         <v>1</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="56">
         <f>SUM(Planilha1!E24)</f>
         <v>9</v>
       </c>
-      <c r="D16" s="57">
+      <c r="D16" s="56">
         <f>SUM(Planilha1!F24)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="57">
         <f>SUM(A16:D16)</f>
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A17" s="56"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="58"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="57"/>
     </row>
     <row r="18" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A18" s="56"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
     </row>
     <row r="19" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A19" s="56"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
     </row>
     <row r="20" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A20" s="56"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
     </row>
     <row r="21" spans="1:10" ht="8.85" customHeight="1">
-      <c r="A21" s="56"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="57"/>
     </row>
     <row r="22" spans="1:10" ht="34.200000000000003" customHeight="1">
-      <c r="A22" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="57">
+      <c r="A22" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="56">
         <f>SUM(Planilha1!P22,Planilha1!D46,Planilha1!P57,Planilha1!D58,)</f>
         <v>8</v>
       </c>
-      <c r="C22" s="57">
+      <c r="C22" s="56">
         <f>SUM(Planilha1!Q22,Planilha1!E46,Planilha1!Q57,Planilha1!E58)</f>
         <v>29</v>
       </c>
-      <c r="D22" s="57">
+      <c r="D22" s="56">
         <f>SUM(Planilha1!R22,Planilha1!F46,Planilha1!R57,Planilha1!F58)</f>
         <v>8</v>
       </c>
-      <c r="E22" s="58">
+      <c r="E22" s="57">
         <f>SUM(A22:D22)</f>
         <v>45</v>
       </c>
       <c r="J22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A23" s="56"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="58"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="57"/>
     </row>
     <row r="24" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A24" s="56"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="57"/>
     </row>
     <row r="25" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A25" s="56"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="57"/>
     </row>
     <row r="26" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A26" s="56"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="57"/>
     </row>
     <row r="27" spans="1:10" ht="10.65" customHeight="1">
-      <c r="A27" s="56"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="28" spans="1:10" ht="58.2" customHeight="1">
-      <c r="A28" s="55" t="str">
+      <c r="A28" s="54" t="str">
         <f ca="1">"Quartel em Alegrete, " &amp; TEXT(TODAY(), "dd \d\e mmmm \d\e e")</f>
-        <v>Quartel em Alegrete, 25 de julho de 2024</v>
-      </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
+        <v>Quartel em Alegrete, 07 de junho de 2025</v>
+      </c>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="21.75" customHeight="1">
       <c r="A29" s="29"/>
@@ -3852,33 +3483,33 @@
       <c r="E29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A30" s="59"/>
-      <c r="B30" s="59"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
     </row>
     <row r="31" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A31" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="48"/>
+      <c r="A31" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="40"/>
       <c r="C31" s="33"/>
-      <c r="D31" s="61" t="s">
-        <v>131</v>
-      </c>
-      <c r="E31" s="61"/>
+      <c r="D31" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="17.399999999999999" customHeight="1">
-      <c r="A32" s="62" t="s">
-        <v>132</v>
-      </c>
-      <c r="B32" s="62"/>
+      <c r="A32" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="52"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="63" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="63"/>
+      <c r="D32" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="53"/>
     </row>
     <row r="33" spans="1:6" ht="20.85" customHeight="1">
       <c r="A33" s="24"/>
@@ -3898,27 +3529,27 @@
     <row r="39" spans="1:6" ht="13.5" customHeight="1"/>
     <row r="41" spans="1:6" ht="14.25" customHeight="1">
       <c r="F41" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="B44" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="B10:B15"/>
@@ -3935,12 +3566,12 @@
     <mergeCell ref="C22:C27"/>
     <mergeCell ref="D22:D27"/>
     <mergeCell ref="E22:E27"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" scale="41" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>